<commit_message>
Optimize security vulnerability checks
</commit_message>
<xml_diff>
--- a/SAG2_Database_update.xlsx
+++ b/SAG2_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3259,6 +3259,43 @@
         <v>334</v>
       </c>
       <c r="I76" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>45762.76107120371</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>400</v>
+      </c>
+      <c r="G77" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H77" t="n">
+        <v>330</v>
+      </c>
+      <c r="I77" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3273,7 +3310,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6328,6 +6365,45 @@
         <v>338</v>
       </c>
       <c r="I78" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45762.72451388889</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x20,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>0x19</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>400</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>568631262647113771663628</t>
+        </is>
+      </c>
+      <c r="H79" t="n">
+        <v>338</v>
+      </c>
+      <c r="I79" t="n">
         <v>25</v>
       </c>
     </row>
@@ -6342,7 +6418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9169,6 +9245,43 @@
         <v>334</v>
       </c>
       <c r="I76" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>45762.79501923611</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x1a,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>400</v>
+      </c>
+      <c r="G77" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H77" t="n">
+        <v>330</v>
+      </c>
+      <c r="I77" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9183,7 +9296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12013,6 +12126,43 @@
         <v>25</v>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>45762.92137438658</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x11,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>0x19</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>400</v>
+      </c>
+      <c r="G77" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H77" t="n">
+        <v>338</v>
+      </c>
+      <c r="I77" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor security vulnerability checks
</commit_message>
<xml_diff>
--- a/SAG2_Database_update.xlsx
+++ b/SAG2_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3333,6 +3333,43 @@
         <v>330</v>
       </c>
       <c r="I78" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45763.7654925</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>400</v>
+      </c>
+      <c r="G79" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H79" t="n">
+        <v>330</v>
+      </c>
+      <c r="I79" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3347,7 +3384,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6480,6 +6517,45 @@
         <v>334</v>
       </c>
       <c r="I80" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45763.72850694445</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x20,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>0x19</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>400</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>568631262647113771663628</t>
+        </is>
+      </c>
+      <c r="H81" t="n">
+        <v>334</v>
+      </c>
+      <c r="I81" t="n">
         <v>25</v>
       </c>
     </row>
@@ -6494,7 +6570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9395,6 +9471,43 @@
         <v>330</v>
       </c>
       <c r="I78" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45763.80038960648</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x1a,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>400</v>
+      </c>
+      <c r="G79" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H79" t="n">
+        <v>330</v>
+      </c>
+      <c r="I79" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9409,7 +9522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12313,6 +12426,43 @@
         <v>25</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45763.92296003472</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x11,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>0x19</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>400</v>
+      </c>
+      <c r="G79" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H79" t="n">
+        <v>338</v>
+      </c>
+      <c r="I79" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>